<commit_message>
0.5d some documentation added
</commit_message>
<xml_diff>
--- a/WeatherStation_01/WeatherStation.xlsx
+++ b/WeatherStation_01/WeatherStation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emchenko\Documents\Arduino\WeatherStation_01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bemchenko\Documents\Arduino\WeatherStation_01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2E0BD7-ECF8-49E1-A371-5D12CBB99742}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC47009E-36D1-4BE9-AC6E-1F66E01A01DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{B0C9A41E-2C7E-4A7A-8B40-CD68F4668925}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{B0C9A41E-2C7E-4A7A-8B40-CD68F4668925}"/>
   </bookViews>
   <sheets>
     <sheet name="list" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="92">
   <si>
     <t>Electrical Parameters</t>
   </si>
@@ -275,15 +277,99 @@
   <si>
     <t>3.3v - 5v</t>
   </si>
+  <si>
+    <t>Внутри шилда</t>
+  </si>
+  <si>
+    <t>Спец. блок</t>
+  </si>
+  <si>
+    <t>Подключение</t>
+  </si>
+  <si>
+    <t>Размещение</t>
+  </si>
+  <si>
+    <t>Шилд</t>
+  </si>
+  <si>
+    <t>SDA</t>
+  </si>
+  <si>
+    <t>SCL</t>
+  </si>
+  <si>
+    <t>DHT pin</t>
+  </si>
+  <si>
+    <t>GND</t>
+  </si>
+  <si>
+    <t>OneWire pin</t>
+  </si>
+  <si>
+    <t>Спец.блок</t>
+  </si>
+  <si>
+    <t>reserve</t>
+  </si>
+  <si>
+    <t>Дождевая площадка1</t>
+  </si>
+  <si>
+    <t>Дождевая площадка2? Видимо пока нет</t>
+  </si>
+  <si>
+    <t>Capacitor pin1</t>
+  </si>
+  <si>
+    <t>Capacitor pin2</t>
+  </si>
+  <si>
+    <t>Thermistor pin1</t>
+  </si>
+  <si>
+    <t>Thermistor pin2</t>
+  </si>
+  <si>
+    <t>Heater pin1</t>
+  </si>
+  <si>
+    <t>Heater pin2</t>
+  </si>
+  <si>
+    <t>UV</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Дождевая площадка2</t>
+  </si>
+  <si>
+    <t>Analog pin</t>
+  </si>
+  <si>
+    <t>3+1</t>
+  </si>
+  <si>
+    <t>2+1</t>
+  </si>
+  <si>
+    <t>Wiring</t>
+  </si>
+  <si>
+    <t>Спец. блок?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -320,8 +406,34 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="7" tint="0.59999389629810485"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -349,6 +461,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -380,7 +510,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -391,7 +521,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -413,6 +543,17 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -793,115 +934,481 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E350CCA7-7452-459E-9649-8BA1D1792C0B}">
-  <dimension ref="A2:B24"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="25.86328125" customWidth="1"/>
+    <col min="2" max="2" width="13.265625" customWidth="1"/>
+    <col min="3" max="3" width="5" customWidth="1"/>
+    <col min="4" max="4" width="22.9296875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="B1" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D2" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J2" s="4"/>
+      <c r="L2" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G3" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="G4" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4" t="s">
+        <v>72</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D5" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5" t="s">
+        <v>69</v>
+      </c>
+      <c r="K5">
+        <v>3</v>
+      </c>
+      <c r="L5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="G6" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6" t="s">
+        <v>70</v>
+      </c>
+      <c r="K6">
+        <v>4</v>
+      </c>
+      <c r="L6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="G7" s="17">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="I7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D8" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="G8" s="17">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>6</v>
+      </c>
+      <c r="I8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="I10" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11" t="s">
+        <v>78</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D12" t="s">
+        <v>76</v>
+      </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
+      <c r="I12" t="s">
+        <v>79</v>
+      </c>
+      <c r="K12">
+        <v>2</v>
+      </c>
+      <c r="L12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>17</v>
       </c>
       <c r="B13" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="H13">
+        <v>3</v>
+      </c>
+      <c r="I13" t="s">
+        <v>80</v>
+      </c>
+      <c r="K13">
+        <v>3</v>
+      </c>
+      <c r="L13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>16</v>
       </c>
       <c r="B14" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="H14">
+        <v>4</v>
+      </c>
+      <c r="I14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>58</v>
       </c>
       <c r="B15" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="H15">
+        <v>5</v>
+      </c>
+      <c r="I15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="H16">
+        <v>6</v>
+      </c>
+      <c r="I16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A17" s="4" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A19" s="4" t="s">
         <v>61</v>
       </c>
       <c r="B19" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D19" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20" t="s">
+        <v>11</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="H21">
+        <v>2</v>
+      </c>
+      <c r="I21" t="s">
+        <v>72</v>
+      </c>
+      <c r="K21">
+        <v>2</v>
+      </c>
+      <c r="L21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="H22">
+        <v>3</v>
+      </c>
+      <c r="I22" t="s">
+        <v>69</v>
+      </c>
+      <c r="K22">
+        <v>3</v>
+      </c>
+      <c r="L22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A23" s="4" t="s">
         <v>60</v>
       </c>
       <c r="B23" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D23" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="H23">
+        <v>4</v>
+      </c>
+      <c r="I23" t="s">
+        <v>70</v>
+      </c>
+      <c r="K23">
+        <v>4</v>
+      </c>
+      <c r="L23" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B24" t="s">
         <v>63</v>
       </c>
+      <c r="H24">
+        <v>5</v>
+      </c>
+      <c r="I24" t="s">
+        <v>71</v>
+      </c>
+      <c r="K24">
+        <v>5</v>
+      </c>
+      <c r="L24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="H25">
+        <v>6</v>
+      </c>
+      <c r="I25" t="s">
+        <v>73</v>
+      </c>
+      <c r="K25">
+        <v>6</v>
+      </c>
+      <c r="L25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="H26">
+        <v>7</v>
+      </c>
+      <c r="I26" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="K26">
+        <v>7</v>
+      </c>
+      <c r="L26" s="15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A27" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="D27" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="H27">
+        <v>8</v>
+      </c>
+      <c r="I27" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="K27">
+        <v>8</v>
+      </c>
+      <c r="L27" s="16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="H28">
+        <v>9</v>
+      </c>
+      <c r="I28" s="15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="H29">
+        <v>10</v>
+      </c>
+      <c r="I29" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="H30">
+        <v>11</v>
+      </c>
+      <c r="I30" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="H31">
+        <v>12</v>
+      </c>
+      <c r="I31" s="15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="H32">
+        <v>13</v>
+      </c>
+      <c r="I32" s="16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="8:9" x14ac:dyDescent="0.45">
+      <c r="H33">
+        <v>14</v>
+      </c>
+      <c r="I33" s="16" t="s">
+        <v>75</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -910,12 +1417,12 @@
   <dimension ref="A4:N56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M35" sqref="M35:N47"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="4" spans="9:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="9:14" x14ac:dyDescent="0.45">
       <c r="I4" s="1" t="s">
         <v>0</v>
       </c>
@@ -923,7 +1430,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="9:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="9:14" x14ac:dyDescent="0.45">
       <c r="I5" s="2" t="s">
         <v>1</v>
       </c>
@@ -934,7 +1441,7 @@
       </c>
       <c r="M5" s="3"/>
     </row>
-    <row r="6" spans="9:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="9:14" x14ac:dyDescent="0.45">
       <c r="I6" s="2" t="s">
         <v>3</v>
       </c>
@@ -945,7 +1452,7 @@
       </c>
       <c r="M6" s="3"/>
     </row>
-    <row r="7" spans="9:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="9:14" x14ac:dyDescent="0.45">
       <c r="I7" s="2" t="s">
         <v>5</v>
       </c>
@@ -959,7 +1466,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="9:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="9:14" x14ac:dyDescent="0.45">
       <c r="I15" t="s">
         <v>20</v>
       </c>
@@ -976,7 +1483,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="9:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="9:14" x14ac:dyDescent="0.45">
       <c r="I16" t="s">
         <v>18</v>
       </c>
@@ -997,7 +1504,7 @@
         <v>3.4285714285714284</v>
       </c>
     </row>
-    <row r="17" spans="9:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I17" t="s">
         <v>19</v>
       </c>
@@ -1018,7 +1525,7 @@
         <v>285.71428571428572</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A35" s="4" t="s">
         <v>21</v>
       </c>
@@ -1029,7 +1536,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="73.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:14" ht="72" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A36" s="7" t="s">
         <v>22</v>
       </c>
@@ -1053,7 +1560,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A37" s="10" t="s">
         <v>25</v>
       </c>
@@ -1079,7 +1586,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A38" s="11">
         <v>100</v>
       </c>
@@ -1105,7 +1612,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A39" s="12">
         <v>75</v>
       </c>
@@ -1131,7 +1638,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A40" s="11">
         <v>60</v>
       </c>
@@ -1157,7 +1664,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A41" s="12">
         <v>50</v>
       </c>
@@ -1183,7 +1690,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A42" s="11">
         <v>0</v>
       </c>
@@ -1209,7 +1716,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G43" s="11">
         <v>25</v>
       </c>
@@ -1223,7 +1730,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G44" s="13">
         <v>30</v>
       </c>
@@ -1237,7 +1744,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G45" s="11">
         <v>35</v>
       </c>
@@ -1251,7 +1758,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G46" s="13">
         <v>40</v>
       </c>
@@ -1265,7 +1772,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G47" s="11">
         <v>45</v>
       </c>
@@ -1279,7 +1786,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:14" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G48" s="13">
         <v>50</v>
       </c>
@@ -1287,7 +1794,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="49" spans="7:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="7:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G49" s="11">
         <v>55</v>
       </c>
@@ -1295,7 +1802,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="50" spans="7:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="7:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G50" s="13">
         <v>60</v>
       </c>
@@ -1303,7 +1810,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="51" spans="7:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="7:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G51" s="11">
         <v>65</v>
       </c>
@@ -1311,7 +1818,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="52" spans="7:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="7:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G52" s="13">
         <v>70</v>
       </c>
@@ -1319,7 +1826,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="53" spans="7:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="7:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G53" s="11">
         <v>75</v>
       </c>
@@ -1327,7 +1834,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="54" spans="7:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="7:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G54" s="13">
         <v>80</v>
       </c>
@@ -1335,7 +1842,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="55" spans="7:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="7:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G55" s="11">
         <v>85</v>
       </c>
@@ -1343,7 +1850,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="56" spans="7:8" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="56" spans="7:8" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>